<commit_message>
made all grades print out in markdown format
</commit_message>
<xml_diff>
--- a/testOfAssignmentGrader/rajeshoo7/rajeshoo7program99Grade.xlsx
+++ b/testOfAssignmentGrader/rajeshoo7/rajeshoo7program99Grade.xlsx
@@ -388,6 +388,9 @@
           <t>part1</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>10</v>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>10</t>
@@ -400,6 +403,9 @@
           <t>part2</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>10</v>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>10</t>
@@ -411,6 +417,9 @@
         <is>
           <t>part3</t>
         </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>

</xml_diff>